<commit_message>
new updates for home page
new updates for home page
</commit_message>
<xml_diff>
--- a/lib_testcase/com.aislend.CategoryPage.xlsx
+++ b/lib_testcase/com.aislend.CategoryPage.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Akash\aislend\CityMarket\lib_testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
+    <workbookView activeTab="1" windowHeight="7905" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Scenario_CategoryPage" sheetId="2" r:id="rId1"/>
-    <sheet name="TC_CategoryPage" sheetId="3" r:id="rId2"/>
-    <sheet name="TC_CategoryPage2" sheetId="1" r:id="rId3"/>
+    <sheet name="Scenario_CategoryPage" r:id="rId1" sheetId="2"/>
+    <sheet name="TC_CategoryPage" r:id="rId2" sheetId="3"/>
+    <sheet name="TC_CategoryPage2" r:id="rId3" sheetId="1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="340">
   <si>
     <t>Action</t>
   </si>
@@ -947,12 +947,120 @@
   </si>
   <si>
     <t>Text Entered successfully: userchandna4269593@mailinator.com</t>
+  </si>
+  <si>
+    <t>VerifyTitle: City Market Norwalk - Online Grocery Supermarket with Home Delivery</t>
+  </si>
+  <si>
+    <t>VerifyElement: null</t>
+  </si>
+  <si>
+    <t>Click: null</t>
+  </si>
+  <si>
+    <t>SetText: Randomemailid</t>
+  </si>
+  <si>
+    <t>SetText: 123456</t>
+  </si>
+  <si>
+    <t>VerifyText: Akash sangal</t>
+  </si>
+  <si>
+    <t>MoveToCategory: Quick &amp; Easy Food Solutions</t>
+  </si>
+  <si>
+    <t>VerifyText: 717 West Ave Norwalk, Connecticut,
+CT 06850 , USA
++1 203-956-0241</t>
+  </si>
+  <si>
+    <t>VerifyText: All Days 7:30 AM – 9:00 PM</t>
+  </si>
+  <si>
+    <t>VerifyText: Copyright © 2018 City Market Norwalk. All rights reserved. Terms Of Use &amp; Privacy Policy</t>
+  </si>
+  <si>
+    <t>VerifyTitle: City Market Norwalk - Terms of Use</t>
+  </si>
+  <si>
+    <t>CloseBrowser: Child</t>
+  </si>
+  <si>
+    <t>VerifyTitle: City Super Market Norwalk - Privacy Policy</t>
+  </si>
+  <si>
+    <t>VerifyNoElement: null</t>
+  </si>
+  <si>
+    <t>VerifyTitle: Offers</t>
+  </si>
+  <si>
+    <t>VerifyTitle: Order online for Quick &amp; Easy Food Solutions, delivery or store pickup|City Market Norwalk</t>
+  </si>
+  <si>
+    <t>HeaderMenuSearch: My Account</t>
+  </si>
+  <si>
+    <t>HeaderMenuSearch: Account Information</t>
+  </si>
+  <si>
+    <t>HeaderMenuSearch: My Orders</t>
+  </si>
+  <si>
+    <t>HeaderMenuSearch: My Saved Cards</t>
+  </si>
+  <si>
+    <t>HeaderMenuSearch: My Wish List</t>
+  </si>
+  <si>
+    <t>HeaderMenuSearch: Delivery Coverage</t>
+  </si>
+  <si>
+    <t>HeaderMenuSearch: Offers</t>
+  </si>
+  <si>
+    <t>HeaderMenuSearch: Sign Out</t>
+  </si>
+  <si>
+    <t>VerifyText: You have no items in your shopping cart.</t>
+  </si>
+  <si>
+    <t>SetText: milk</t>
+  </si>
+  <si>
+    <t>SearchProduct: Skim Plus 100% Fat Free Milk</t>
+  </si>
+  <si>
+    <t>SetText: asdasd@</t>
+  </si>
+  <si>
+    <t>VerifyText: Please enter a valid email address (Ex: johndoe@domain.com).</t>
+  </si>
+  <si>
+    <t>SetText: asdasd@assdcsadsaasd.com</t>
+  </si>
+  <si>
+    <t>VerifyText: Thank you for your subscription.</t>
+  </si>
+  <si>
+    <t>VerifyCategoryAndProduct: null</t>
+  </si>
+  <si>
+    <t>VerifySiteMapFromCategoryPage: null</t>
+  </si>
+  <si>
+    <t>VerifyFooterLinks: null</t>
+  </si>
+  <si>
+    <t>Wait: 6000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -1095,55 +1203,55 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="2">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="4" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="4" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="4" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="2">
@@ -1170,10 +1278,10 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+  <tableStyles count="1" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2">
+    <tableStyle count="2" name="MySqlDefault" pivot="0" table="0">
+      <tableStyleElement dxfId="1" type="wholeTable"/>
+      <tableStyleElement dxfId="0" type="headerRow"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1192,10 +1300,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1230,7 +1338,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1265,7 +1373,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1359,21 +1467,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1390,7 +1498,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1442,14 +1550,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
@@ -1458,13 +1566,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="5" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="57.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="36.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.140625" style="5" collapsed="1"/>
-    <col min="6" max="6" width="49.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="5" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="57.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="13.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="36.42578125" collapsed="true"/>
+    <col min="5" max="5" style="5" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="5" width="49.85546875" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1660,35 +1768,35 @@
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="A1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C63" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C63" workbookViewId="0" zoomScale="60" zoomScaleNormal="60">
       <selection activeCell="A66" sqref="A66:O69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="44.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="10" width="23.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="24.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="20.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="44.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="18.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="20.7109375" collapsed="true"/>
+    <col min="6" max="10" customWidth="true" style="1" width="23.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="24.5703125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="20.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="1" width="11.140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="18.7109375" collapsed="true"/>
+    <col min="16" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="30">
+    <row customFormat="1" ht="30" r="1" s="2" spans="1:15">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -1735,7 +1843,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="75">
+    <row ht="75" r="2" spans="1:15">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -1760,7 +1868,7 @@
         <v>68</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>21</v>
@@ -1772,7 +1880,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="30">
+    <row ht="30" r="3" spans="1:15">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -1799,7 +1907,7 @@
         <v>69</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>42</v>
+        <v>306</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>21</v>
@@ -1811,7 +1919,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="30">
+    <row ht="30" r="4" spans="1:15">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -1838,7 +1946,7 @@
         <v>70</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>21</v>
@@ -1850,7 +1958,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="45">
+    <row ht="45" r="5" spans="1:15">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -1877,7 +1985,7 @@
         <v>71</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>42</v>
+        <v>306</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>21</v>
@@ -1889,7 +1997,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="30">
+    <row ht="30" r="6" spans="1:15">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -1922,7 +2030,7 @@
         <v>74</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>21</v>
@@ -1934,7 +2042,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="30">
+    <row ht="30" r="7" spans="1:15">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -1963,7 +2071,7 @@
         <v>73</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>67</v>
+        <v>309</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>21</v>
@@ -1975,7 +2083,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="30">
+    <row ht="30" r="8" spans="1:15">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -2002,7 +2110,7 @@
         <v>72</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>21</v>
@@ -2014,7 +2122,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="45">
+    <row ht="45" r="9" spans="1:15">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -2043,7 +2151,7 @@
         <v>75</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>249</v>
+        <v>310</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>21</v>
@@ -2055,7 +2163,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="75">
+    <row ht="75" r="10" spans="1:15">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -2080,7 +2188,7 @@
         <v>68</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>21</v>
@@ -2092,7 +2200,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="60">
+    <row ht="60" r="11" spans="1:15">
       <c r="A11" s="4" t="s">
         <v>45</v>
       </c>
@@ -2121,7 +2229,7 @@
         <v>239</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>250</v>
+        <v>311</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>21</v>
@@ -2133,7 +2241,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="75">
+    <row ht="75" r="12" spans="1:15">
       <c r="A12" s="4" t="s">
         <v>45</v>
       </c>
@@ -2160,7 +2268,7 @@
         <v>98</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>42</v>
+        <v>306</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>21</v>
@@ -2172,7 +2280,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="45">
+    <row ht="45" r="13" spans="1:15">
       <c r="A13" s="4" t="s">
         <v>45</v>
       </c>
@@ -2199,7 +2307,7 @@
         <v>99</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>42</v>
+        <v>306</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>21</v>
@@ -2211,7 +2319,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="30">
+    <row ht="30" r="14" spans="1:15">
       <c r="A14" s="4" t="s">
         <v>45</v>
       </c>
@@ -2238,7 +2346,7 @@
         <v>103</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>42</v>
+        <v>306</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>21</v>
@@ -2250,7 +2358,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="45">
+    <row ht="45" r="15" spans="1:15">
       <c r="A15" s="4" t="s">
         <v>45</v>
       </c>
@@ -2277,7 +2385,7 @@
         <v>104</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>42</v>
+        <v>306</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>21</v>
@@ -2289,7 +2397,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="45">
+    <row ht="45" r="16" spans="1:15">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
@@ -2316,7 +2424,7 @@
         <v>100</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>42</v>
+        <v>306</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>21</v>
@@ -2328,7 +2436,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="30">
+    <row ht="30" r="17" spans="1:15">
       <c r="A17" s="4" t="s">
         <v>45</v>
       </c>
@@ -2355,7 +2463,7 @@
         <v>101</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>42</v>
+        <v>306</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>21</v>
@@ -2367,7 +2475,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="75">
+    <row ht="75" r="18" spans="1:15">
       <c r="A18" s="4" t="s">
         <v>45</v>
       </c>
@@ -2394,7 +2502,7 @@
         <v>102</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>42</v>
+        <v>306</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>21</v>
@@ -2406,7 +2514,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="75">
+    <row ht="75" r="19" spans="1:15">
       <c r="A19" s="4" t="s">
         <v>45</v>
       </c>
@@ -2435,7 +2543,7 @@
         <v>111</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>223</v>
+        <v>312</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>21</v>
@@ -2447,7 +2555,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="45">
+    <row ht="45" r="20" spans="1:15">
       <c r="A20" s="4" t="s">
         <v>45</v>
       </c>
@@ -2476,7 +2584,7 @@
         <v>112</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>224</v>
+        <v>313</v>
       </c>
       <c r="M20" s="4" t="s">
         <v>21</v>
@@ -2488,7 +2596,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="90">
+    <row ht="90" r="21" spans="1:15">
       <c r="A21" s="4" t="s">
         <v>45</v>
       </c>
@@ -2517,7 +2625,7 @@
         <v>123</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>225</v>
+        <v>314</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>21</v>
@@ -2529,7 +2637,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="45">
+    <row ht="45" r="22" spans="1:15">
       <c r="A22" s="4" t="s">
         <v>45</v>
       </c>
@@ -2556,7 +2664,7 @@
         <v>124</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>21</v>
@@ -2568,7 +2676,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="45">
+    <row ht="45" r="23" spans="1:15">
       <c r="A23" s="4" t="s">
         <v>45</v>
       </c>
@@ -2595,7 +2703,7 @@
         <v>125</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>21</v>
@@ -2607,7 +2715,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="30">
+    <row ht="30" r="24" spans="1:15">
       <c r="A24" s="4" t="s">
         <v>45</v>
       </c>
@@ -2632,7 +2740,7 @@
         <v>126</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>226</v>
+        <v>316</v>
       </c>
       <c r="M24" s="4" t="s">
         <v>21</v>
@@ -2644,7 +2752,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="45">
+    <row ht="45" r="25" spans="1:15">
       <c r="A25" s="4" t="s">
         <v>45</v>
       </c>
@@ -2671,7 +2779,7 @@
         <v>127</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="M25" s="4" t="s">
         <v>21</v>
@@ -2683,7 +2791,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="45">
+    <row ht="45" r="26" spans="1:15">
       <c r="A26" s="4" t="s">
         <v>45</v>
       </c>
@@ -2710,7 +2818,7 @@
         <v>128</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>296</v>
+        <v>317</v>
       </c>
       <c r="M26" s="4" t="s">
         <v>21</v>
@@ -2722,7 +2830,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="30">
+    <row ht="30" r="27" spans="1:15">
       <c r="A27" s="4" t="s">
         <v>45</v>
       </c>
@@ -2747,7 +2855,7 @@
         <v>129</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>226</v>
+        <v>316</v>
       </c>
       <c r="M27" s="4" t="s">
         <v>21</v>
@@ -2759,7 +2867,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="45">
+    <row ht="45" r="28" spans="1:15">
       <c r="A28" s="4" t="s">
         <v>46</v>
       </c>
@@ -2786,7 +2894,7 @@
         <v>139</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="M28" s="4" t="s">
         <v>21</v>
@@ -2798,7 +2906,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="45">
+    <row ht="45" r="29" spans="1:15">
       <c r="A29" s="4" t="s">
         <v>46</v>
       </c>
@@ -2825,7 +2933,7 @@
         <v>138</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>42</v>
+        <v>306</v>
       </c>
       <c r="M29" s="4" t="s">
         <v>21</v>
@@ -2837,7 +2945,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="45">
+    <row ht="45" r="30" spans="1:15">
       <c r="A30" s="4" t="s">
         <v>46</v>
       </c>
@@ -2864,7 +2972,7 @@
         <v>140</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="M30" s="4" t="s">
         <v>21</v>
@@ -2876,7 +2984,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="45">
+    <row ht="45" r="31" spans="1:15">
       <c r="A31" s="4" t="s">
         <v>46</v>
       </c>
@@ -2903,7 +3011,7 @@
         <v>142</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>42</v>
+        <v>318</v>
       </c>
       <c r="M31" s="4" t="s">
         <v>21</v>
@@ -2915,7 +3023,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="45">
+    <row ht="45" r="32" spans="1:15">
       <c r="A32" s="4" t="s">
         <v>47</v>
       </c>
@@ -2942,7 +3050,7 @@
         <v>151</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="M32" s="4" t="s">
         <v>21</v>
@@ -2954,7 +3062,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="30">
+    <row ht="30" r="33" spans="1:15">
       <c r="A33" s="4" t="s">
         <v>47</v>
       </c>
@@ -2979,7 +3087,7 @@
         <v>152</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>280</v>
+        <v>319</v>
       </c>
       <c r="M33" s="4" t="s">
         <v>21</v>
@@ -2991,7 +3099,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="60">
+    <row ht="60" r="34" spans="1:15">
       <c r="A34" s="4" t="s">
         <v>47</v>
       </c>
@@ -3020,7 +3128,7 @@
         <v>153</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>250</v>
+        <v>311</v>
       </c>
       <c r="M34" s="4" t="s">
         <v>21</v>
@@ -3032,7 +3140,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="90">
+    <row ht="90" r="35" spans="1:15">
       <c r="A35" s="4" t="s">
         <v>47</v>
       </c>
@@ -3057,7 +3165,7 @@
         <v>154</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>297</v>
+        <v>320</v>
       </c>
       <c r="M35" s="4" t="s">
         <v>21</v>
@@ -3069,7 +3177,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="45">
+    <row ht="45" r="36" spans="1:15">
       <c r="A36" s="4" t="s">
         <v>48</v>
       </c>
@@ -3096,7 +3204,7 @@
         <v>139</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="M36" s="4" t="s">
         <v>21</v>
@@ -3108,7 +3216,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="45">
+    <row ht="45" r="37" spans="1:15">
       <c r="A37" s="4" t="s">
         <v>48</v>
       </c>
@@ -3133,7 +3241,7 @@
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4" t="s">
-        <v>42</v>
+        <v>306</v>
       </c>
       <c r="M37" s="4" t="s">
         <v>21</v>
@@ -3145,7 +3253,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="45">
+    <row ht="45" r="38" spans="1:15">
       <c r="A38" s="4" t="s">
         <v>48</v>
       </c>
@@ -3174,7 +3282,7 @@
         <v>157</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>281</v>
+        <v>321</v>
       </c>
       <c r="M38" s="4" t="s">
         <v>21</v>
@@ -3186,7 +3294,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="45">
+    <row ht="45" r="39" spans="1:15">
       <c r="A39" s="4" t="s">
         <v>48</v>
       </c>
@@ -3215,7 +3323,7 @@
         <v>167</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>282</v>
+        <v>322</v>
       </c>
       <c r="M39" s="4" t="s">
         <v>21</v>
@@ -3227,7 +3335,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="45">
+    <row ht="45" r="40" spans="1:15">
       <c r="A40" s="4" t="s">
         <v>48</v>
       </c>
@@ -3256,7 +3364,7 @@
         <v>169</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>283</v>
+        <v>323</v>
       </c>
       <c r="M40" s="4" t="s">
         <v>21</v>
@@ -3268,7 +3376,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="45">
+    <row ht="45" r="41" spans="1:15">
       <c r="A41" s="4" t="s">
         <v>48</v>
       </c>
@@ -3297,7 +3405,7 @@
         <v>171</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>284</v>
+        <v>324</v>
       </c>
       <c r="M41" s="4" t="s">
         <v>21</v>
@@ -3309,7 +3417,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="45">
+    <row ht="45" r="42" spans="1:15">
       <c r="A42" s="4" t="s">
         <v>48</v>
       </c>
@@ -3338,7 +3446,7 @@
         <v>173</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>285</v>
+        <v>325</v>
       </c>
       <c r="M42" s="4" t="s">
         <v>21</v>
@@ -3350,7 +3458,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="45">
+    <row ht="45" r="43" spans="1:15">
       <c r="A43" s="4" t="s">
         <v>48</v>
       </c>
@@ -3379,7 +3487,7 @@
         <v>175</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>286</v>
+        <v>326</v>
       </c>
       <c r="M43" s="4" t="s">
         <v>21</v>
@@ -3391,7 +3499,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="45">
+    <row ht="45" r="44" spans="1:15">
       <c r="A44" s="4" t="s">
         <v>48</v>
       </c>
@@ -3420,7 +3528,7 @@
         <v>177</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>287</v>
+        <v>327</v>
       </c>
       <c r="M44" s="4" t="s">
         <v>21</v>
@@ -3432,7 +3540,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="45">
+    <row ht="45" r="45" spans="1:15">
       <c r="A45" s="4" t="s">
         <v>48</v>
       </c>
@@ -3461,7 +3569,7 @@
         <v>179</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>288</v>
+        <v>328</v>
       </c>
       <c r="M45" s="4" t="s">
         <v>21</v>
@@ -3473,7 +3581,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="30">
+    <row ht="30" r="46" spans="1:15">
       <c r="A46" s="4" t="s">
         <v>48</v>
       </c>
@@ -3500,7 +3608,7 @@
         <v>185</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="M46" s="4" t="s">
         <v>21</v>
@@ -3512,7 +3620,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="45">
+    <row ht="45" r="47" spans="1:15">
       <c r="A47" s="4" t="s">
         <v>48</v>
       </c>
@@ -3539,7 +3647,7 @@
         <v>181</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>42</v>
+        <v>318</v>
       </c>
       <c r="M47" s="4" t="s">
         <v>21</v>
@@ -3551,7 +3659,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="60">
+    <row ht="60" r="48" spans="1:15">
       <c r="A48" s="4" t="s">
         <v>49</v>
       </c>
@@ -3578,7 +3686,7 @@
         <v>198</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="M48" s="4" t="s">
         <v>21</v>
@@ -3590,7 +3698,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="75">
+    <row ht="75" r="49" spans="1:15">
       <c r="A49" s="4" t="s">
         <v>49</v>
       </c>
@@ -3617,7 +3725,7 @@
         <v>196</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>42</v>
+        <v>306</v>
       </c>
       <c r="M49" s="4" t="s">
         <v>21</v>
@@ -3629,7 +3737,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="60">
+    <row ht="60" r="50" spans="1:15">
       <c r="A50" s="4" t="s">
         <v>49</v>
       </c>
@@ -3658,7 +3766,7 @@
         <v>197</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>251</v>
+        <v>329</v>
       </c>
       <c r="M50" s="4" t="s">
         <v>21</v>
@@ -3670,7 +3778,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="30">
+    <row ht="30" r="51" spans="1:15">
       <c r="A51" s="4" t="s">
         <v>49</v>
       </c>
@@ -3697,7 +3805,7 @@
         <v>198</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="M51" s="4" t="s">
         <v>21</v>
@@ -3709,7 +3817,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="75">
+    <row ht="75" r="52" spans="1:15">
       <c r="A52" s="4" t="s">
         <v>49</v>
       </c>
@@ -3736,7 +3844,7 @@
         <v>199</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>42</v>
+        <v>318</v>
       </c>
       <c r="M52" s="4" t="s">
         <v>21</v>
@@ -3748,7 +3856,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="30">
+    <row ht="30" r="53" spans="1:15">
       <c r="A53" s="4" t="s">
         <v>50</v>
       </c>
@@ -3777,7 +3885,7 @@
         <v>202</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>252</v>
+        <v>330</v>
       </c>
       <c r="M53" s="4" t="s">
         <v>21</v>
@@ -3789,7 +3897,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="45">
+    <row ht="45" r="54" spans="1:15">
       <c r="A54" s="4" t="s">
         <v>50</v>
       </c>
@@ -3816,7 +3924,7 @@
         <v>205</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="M54" s="4" t="s">
         <v>21</v>
@@ -3828,7 +3936,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="75">
+    <row ht="75" r="55" spans="1:15">
       <c r="A55" s="4" t="s">
         <v>50</v>
       </c>
@@ -3857,7 +3965,7 @@
         <v>209</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>253</v>
+        <v>331</v>
       </c>
       <c r="M55" s="4" t="s">
         <v>21</v>
@@ -3869,7 +3977,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="60">
+    <row ht="60" r="56" spans="1:15">
       <c r="A56" s="4" t="s">
         <v>50</v>
       </c>
@@ -3898,7 +4006,7 @@
         <v>153</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>250</v>
+        <v>311</v>
       </c>
       <c r="M56" s="4" t="s">
         <v>21</v>
@@ -3910,7 +4018,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="30">
+    <row ht="30" r="57" spans="1:15">
       <c r="A57" s="4" t="s">
         <v>51</v>
       </c>
@@ -3939,7 +4047,7 @@
         <v>220</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>263</v>
+        <v>332</v>
       </c>
       <c r="M57" s="4" t="s">
         <v>21</v>
@@ -3951,7 +4059,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="45">
+    <row ht="45" r="58" spans="1:15">
       <c r="A58" s="4" t="s">
         <v>51</v>
       </c>
@@ -3978,7 +4086,7 @@
         <v>221</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="M58" s="4" t="s">
         <v>21</v>
@@ -3990,7 +4098,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="75">
+    <row ht="75" r="59" spans="1:15">
       <c r="A59" s="4" t="s">
         <v>51</v>
       </c>
@@ -4019,7 +4127,7 @@
         <v>267</v>
       </c>
       <c r="L59" s="4" t="s">
-        <v>268</v>
+        <v>333</v>
       </c>
       <c r="M59" s="4" t="s">
         <v>21</v>
@@ -4031,7 +4139,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="45">
+    <row ht="45" r="60" spans="1:15">
       <c r="A60" s="4" t="s">
         <v>51</v>
       </c>
@@ -4060,7 +4168,7 @@
         <v>220</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>254</v>
+        <v>334</v>
       </c>
       <c r="M60" s="4" t="s">
         <v>21</v>
@@ -4072,7 +4180,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="45">
+    <row ht="45" r="61" spans="1:15">
       <c r="A61" s="4" t="s">
         <v>51</v>
       </c>
@@ -4099,7 +4207,7 @@
         <v>221</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="M61" s="4" t="s">
         <v>21</v>
@@ -4111,7 +4219,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="60">
+    <row ht="60" r="62" spans="1:15">
       <c r="A62" s="4" t="s">
         <v>51</v>
       </c>
@@ -4140,7 +4248,7 @@
         <v>222</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>299</v>
+        <v>335</v>
       </c>
       <c r="M62" s="4" t="s">
         <v>21</v>
@@ -4152,7 +4260,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="60">
+    <row ht="60" r="63" spans="1:15">
       <c r="A63" s="4" t="s">
         <v>52</v>
       </c>
@@ -4179,7 +4287,7 @@
         <v>229</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>289</v>
+        <v>336</v>
       </c>
       <c r="M63" s="4" t="s">
         <v>21</v>
@@ -4191,7 +4299,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="60">
+    <row ht="60" r="64" spans="1:15">
       <c r="A64" s="4" t="s">
         <v>53</v>
       </c>
@@ -4218,7 +4326,7 @@
         <v>229</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>298</v>
+        <v>337</v>
       </c>
       <c r="M64" s="4" t="s">
         <v>21</v>
@@ -4230,7 +4338,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="45">
+    <row ht="45" r="65" spans="1:15">
       <c r="A65" s="4" t="s">
         <v>271</v>
       </c>
@@ -4257,7 +4365,7 @@
         <v>279</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>290</v>
+        <v>338</v>
       </c>
       <c r="M65" s="4" t="s">
         <v>21</v>
@@ -4269,7 +4377,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="30">
+    <row ht="30" r="66" spans="1:15">
       <c r="A66" s="4" t="s">
         <v>274</v>
       </c>
@@ -4296,7 +4404,7 @@
         <v>232</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="M66" s="4" t="s">
         <v>21</v>
@@ -4308,7 +4416,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="30">
+    <row ht="30" r="67" spans="1:15">
       <c r="A67" s="4" t="s">
         <v>274</v>
       </c>
@@ -4335,7 +4443,7 @@
         <v>235</v>
       </c>
       <c r="L67" s="4" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="M67" s="4" t="s">
         <v>21</v>
@@ -4347,7 +4455,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="30">
+    <row ht="30" r="68" spans="1:15">
       <c r="A68" s="4" t="s">
         <v>274</v>
       </c>
@@ -4370,7 +4478,7 @@
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
       <c r="L68" s="4" t="s">
-        <v>255</v>
+        <v>339</v>
       </c>
       <c r="M68" s="4" t="s">
         <v>21</v>
@@ -4382,7 +4490,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="45">
+    <row ht="45" r="69" spans="1:15">
       <c r="A69" s="4" t="s">
         <v>274</v>
       </c>
@@ -4409,7 +4517,7 @@
         <v>69</v>
       </c>
       <c r="L69" s="4" t="s">
-        <v>42</v>
+        <v>306</v>
       </c>
       <c r="M69" s="4" t="s">
         <v>21</v>
@@ -4423,38 +4531,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G57" r:id="rId1"/>
-    <hyperlink ref="H6" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="G57"/>
+    <hyperlink r:id="rId2" ref="H6"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="60" zoomScaleNormal="60">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="44.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="10" width="23.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="24.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="20.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="44.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="18.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="20.7109375" collapsed="true"/>
+    <col min="6" max="10" customWidth="true" style="1" width="23.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="24.5703125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="20.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="1" width="11.140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="18.7109375" collapsed="true"/>
+    <col min="16" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="30">
+    <row customFormat="1" ht="30" r="1" s="2" spans="1:15">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -4501,7 +4609,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="75">
+    <row ht="75" r="2" spans="1:15">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -4538,7 +4646,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="30">
+    <row ht="30" r="3" spans="1:15">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -4577,7 +4685,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="30">
+    <row ht="30" r="4" spans="1:15">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -4616,7 +4724,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="45">
+    <row ht="45" r="5" spans="1:15">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -4655,7 +4763,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="45">
+    <row ht="45" r="6" spans="1:15">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -4700,7 +4808,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="30">
+    <row ht="30" r="7" spans="1:15">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -4741,7 +4849,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="30">
+    <row ht="30" r="8" spans="1:15">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -4780,7 +4888,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="30">
+    <row ht="30" r="9" spans="1:15">
       <c r="A9" s="4" t="s">
         <v>274</v>
       </c>
@@ -4819,7 +4927,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="30">
+    <row ht="30" r="10" spans="1:15">
       <c r="A10" s="4" t="s">
         <v>274</v>
       </c>
@@ -4858,7 +4966,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="30">
+    <row ht="30" r="11" spans="1:15">
       <c r="A11" s="4" t="s">
         <v>274</v>
       </c>
@@ -4893,7 +5001,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="45">
+    <row ht="45" r="12" spans="1:15">
       <c r="A12" s="4" t="s">
         <v>274</v>
       </c>
@@ -4934,9 +5042,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1"/>
+    <hyperlink r:id="rId1" ref="H6"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mini cart product erification updates
mini cart product erification updates
</commit_message>
<xml_diff>
--- a/lib_testcase/com.aislend.CategoryPage.xlsx
+++ b/lib_testcase/com.aislend.CategoryPage.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2790" uniqueCount="348">
   <si>
     <t>Action</t>
   </si>
@@ -1057,6 +1057,67 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>action VerifySiteMapFromCategoryPage failed: null  null</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//ul[normalize-space(@class) = 'nav-primary mmenu__parent-list']"}
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 39 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 61816d28be1bbd78b3d2429a87a9572e
+*** Element info: {Using=xpath, value=//ul[normalize-space(@class) = 'nav-primary mmenu__parent-list']}</t>
+  </si>
+  <si>
+    <t>action VerifyFooterLinks failed</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//div[normalize-space(@class) = 'footer__inner-left']"}
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 25 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 61816d28be1bbd78b3d2429a87a9572e
+*** Element info: {Using=xpath, value=//div[normalize-space(@class) = 'footer__inner-left']}</t>
+  </si>
+  <si>
+    <t>action click failed</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//span[contains(text(),'Akash')]"}
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 24 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 61816d28be1bbd78b3d2429a87a9572e
+*** Element info: {Using=xpath, value=//span[contains(text(),'Akash')]}</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//a[contains(text(),'Sign Out')]"}
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 28 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 61816d28be1bbd78b3d2429a87a9572e
+*** Element info: {Using=xpath, value=//a[contains(text(),'Sign Out')]}</t>
   </si>
 </sst>
 </file>
@@ -4293,7 +4354,7 @@
         <v>336</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>340</v>
+        <v>21</v>
       </c>
       <c r="N63" s="4" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
new request for changes on master
</commit_message>
<xml_diff>
--- a/lib_testcase/com.aislend.CategoryPage.xlsx
+++ b/lib_testcase/com.aislend.CategoryPage.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4647" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5259" uniqueCount="357">
   <si>
     <t>Action</t>
   </si>
@@ -1176,6 +1176,45 @@
 Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir10312_28400}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
 Session ID: f2cebe5091e466e18a4be64df33544d9
 *** Element info: {Using=id, value=magestore-button-sociallogin}</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//div[normalize-space(@class) = 'footer__inner-left']"}
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 16 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.29.134', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir13728_20410}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: f603c9ae853f4b702e5e6ab2637cdcb2
+*** Element info: {Using=xpath, value=//div[normalize-space(@class) = 'footer__inner-left']}</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//span[contains(text(),'Akash')]"}
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 16 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.29.134', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir13728_20410}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: f603c9ae853f4b702e5e6ab2637cdcb2
+*** Element info: {Using=xpath, value=//span[contains(text(),'Akash')]}</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//a[contains(text(),'Sign Out')]"}
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 16 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.29.134', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir13728_20410}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: f603c9ae853f4b702e5e6ab2637cdcb2
+*** Element info: {Using=xpath, value=//a[contains(text(),'Sign Out')]}</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
implementation of QC reports
implementation of QC reports
</commit_message>
<xml_diff>
--- a/lib_testcase/com.aislend.CategoryPage.xlsx
+++ b/lib_testcase/com.aislend.CategoryPage.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5259" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5913" uniqueCount="369">
   <si>
     <t>Action</t>
   </si>
@@ -1215,6 +1215,109 @@
 Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir13728_20410}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
 Session ID: f603c9ae853f4b702e5e6ab2637cdcb2
 *** Element info: {Using=xpath, value=//a[contains(text(),'Sign Out')]}</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//a[contains(text(),'My Account')]"}
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 15 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir15604_25552}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 285dfc6c4ff02f19aa04f0a8aca12f47
+*** Element info: {Using=xpath, value=//a[contains(text(),'My Account')]}</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"id","selector":"magestore-sociallogin-popup-email"}
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 22 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir15604_25552}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 285dfc6c4ff02f19aa04f0a8aca12f47
+*** Element info: {Using=id, value=magestore-sociallogin-popup-email}</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"id","selector":"magestore-sociallogin-popup-pass"}
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 20 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir15604_25552}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 285dfc6c4ff02f19aa04f0a8aca12f47
+*** Element info: {Using=id, value=magestore-sociallogin-popup-pass}</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"id","selector":"magestore-button-sociallogin"}
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 22 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir15604_25552}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 285dfc6c4ff02f19aa04f0a8aca12f47
+*** Element info: {Using=id, value=magestore-button-sociallogin}</t>
+  </si>
+  <si>
+    <t>text not verified: Akash sangal</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for presence of element located by: By.xpath: //span[contains(text(),'Akash')] (tried for 40 second(s) with 500 MILLISECONDS interval)
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir15604_25552}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 285dfc6c4ff02f19aa04f0a8aca12f47</t>
+  </si>
+  <si>
+    <t>action MoveToCategory failed: Quick &amp; Easy Food Solutions</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//ul[normalize-space(@class) = 'nav-primary mmenu__parent-list']"}
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 14 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir15604_25552}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 285dfc6c4ff02f19aa04f0a8aca12f47
+*** Element info: {Using=xpath, value=//ul[normalize-space(@class) = 'nav-primary mmenu__parent-list']}</t>
+  </si>
+  <si>
+    <t>text not verified: 717 West Ave Norwalk, Connecticut,
+CT 06850 , USA
++1 203-956-0241</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for presence of element located by: By.xpath: //div[normalize-space(@class) = 'footer__location-phone'] (tried for 40 second(s) with 500 MILLISECONDS interval)
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir15604_25552}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 285dfc6c4ff02f19aa04f0a8aca12f47</t>
+  </si>
+  <si>
+    <t>text not verified: All Days 7:30 AM – 9:00 PM</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for presence of element located by: By.xpath: //div[normalize-space(@class) = 'footer-time-slot'] (tried for 40 second(s) with 500 MILLISECONDS interval)
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir15604_25552}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 285dfc6c4ff02f19aa04f0a8aca12f47</t>
   </si>
 </sst>
 </file>

</xml_diff>